<commit_message>
Added Software Requirement Specification.docx
</commit_message>
<xml_diff>
--- a/CSPROJ/Agile Activity List.xlsx
+++ b/CSPROJ/Agile Activity List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -542,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -864,15 +864,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>

</xml_diff>